<commit_message>
final version for manuscript
</commit_message>
<xml_diff>
--- a/landmarks/torso_landmarks.xlsx
+++ b/landmarks/torso_landmarks.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIPAG_~1\AppData\Local\Temp\Mxt214\RemoteFiles\66984_7_65\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MIPAG_~1\AppData\Local\Temp\Mxt214\RemoteFiles\263658_2_53\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="693" uniqueCount="120">
   <si>
     <t>Cohort</t>
   </si>
@@ -309,9 +309,6 @@
   </si>
   <si>
     <t>DICOM Location</t>
-  </si>
-  <si>
-    <t>TLC</t>
   </si>
   <si>
     <t>Expn</t>
@@ -407,6 +404,9 @@
   <si>
     <t>ei dist
 (mm)</t>
+  </si>
+  <si>
+    <t>Scaled up all by ---&gt;</t>
   </si>
 </sst>
 </file>
@@ -1060,13 +1060,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U170"/>
+  <dimension ref="A1:V170"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <pane xSplit="3" ySplit="1" topLeftCell="J2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="1" topLeftCell="D45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T22" sqref="T22"/>
+      <selection pane="bottomRight" activeCell="V65" sqref="V65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1106,50 +1106,50 @@
         <v>91</v>
       </c>
       <c r="F1" s="21" t="s">
+        <v>94</v>
+      </c>
+      <c r="G1" s="21" t="s">
+        <v>99</v>
+      </c>
+      <c r="H1" s="21" t="s">
+        <v>98</v>
+      </c>
+      <c r="I1" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="G1" s="21" t="s">
-        <v>100</v>
-      </c>
-      <c r="H1" s="21" t="s">
-        <v>99</v>
-      </c>
-      <c r="I1" s="22" t="s">
+      <c r="J1" s="22" t="s">
+        <v>97</v>
+      </c>
+      <c r="K1" s="22" t="s">
         <v>96</v>
       </c>
-      <c r="J1" s="22" t="s">
-        <v>98</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>97</v>
-      </c>
       <c r="L1" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" s="45" t="s">
+        <v>106</v>
+      </c>
+      <c r="N1" s="39" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" s="39" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="45" t="s">
         <v>103</v>
       </c>
-      <c r="M1" s="45" t="s">
-        <v>107</v>
-      </c>
-      <c r="N1" s="39" t="s">
-        <v>108</v>
-      </c>
-      <c r="O1" s="39" t="s">
-        <v>109</v>
-      </c>
-      <c r="P1" s="45" t="s">
+      <c r="Q1" s="39" t="s">
         <v>104</v>
       </c>
-      <c r="Q1" s="39" t="s">
+      <c r="R1" s="39" t="s">
         <v>105</v>
-      </c>
-      <c r="R1" s="39" t="s">
-        <v>106</v>
       </c>
       <c r="S1" s="46"/>
       <c r="T1" s="10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="U1" s="9" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
@@ -1163,7 +1163,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F2" s="23">
         <v>768</v>
@@ -1184,7 +1184,7 @@
         <v>0.5</v>
       </c>
       <c r="L2" s="51" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="M2" s="43">
         <v>162</v>
@@ -1210,6 +1210,9 @@
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
@@ -1220,7 +1223,7 @@
         <v>2</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F3" s="23">
         <v>768</v>
@@ -1241,7 +1244,7 @@
         <v>0.5</v>
       </c>
       <c r="L3" s="51" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="M3" s="50">
         <v>41</v>
@@ -1259,10 +1262,10 @@
         <v>411</v>
       </c>
       <c r="R3" s="15">
-        <v>394</v>
+        <v>414</v>
       </c>
       <c r="T3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="U3" s="70">
         <f t="shared" ref="U3:U48" si="0">(P3-M3)*K3</f>
@@ -1280,7 +1283,7 @@
         <v>2</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F4" s="23">
         <v>768</v>
@@ -1335,7 +1338,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F5" s="23">
         <v>768</v>
@@ -1389,7 +1392,7 @@
         <v>2</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F6" s="23">
         <v>768</v>
@@ -1443,7 +1446,7 @@
         <v>2</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F7" s="23">
         <v>768</v>
@@ -1497,7 +1500,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F8" s="23">
         <v>768</v>
@@ -1551,7 +1554,7 @@
         <v>2</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F9" s="23">
         <v>768</v>
@@ -1605,7 +1608,7 @@
         <v>2</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F10" s="23">
         <v>768</v>
@@ -1659,7 +1662,7 @@
         <v>2</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F11" s="23">
         <v>768</v>
@@ -1713,7 +1716,7 @@
         <v>2</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F12" s="23">
         <v>768</v>
@@ -1768,7 +1771,7 @@
         <v>2</v>
       </c>
       <c r="E13" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F13" s="23">
         <v>768</v>
@@ -1822,7 +1825,7 @@
         <v>2</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F14" s="23">
         <v>768</v>
@@ -1876,7 +1879,7 @@
         <v>2</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F15" s="23">
         <v>768</v>
@@ -1930,7 +1933,7 @@
         <v>2</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F16" s="23">
         <v>768</v>
@@ -1984,7 +1987,7 @@
         <v>2</v>
       </c>
       <c r="E17" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F17" s="23">
         <v>768</v>
@@ -2038,7 +2041,7 @@
         <v>2</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F18" s="23">
         <v>768</v>
@@ -2092,7 +2095,7 @@
         <v>2</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F19" s="23">
         <v>768</v>
@@ -2146,7 +2149,7 @@
         <v>2</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F20" s="23">
         <v>768</v>
@@ -2200,7 +2203,7 @@
         <v>2</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F21" s="23">
         <v>768</v>
@@ -2254,7 +2257,7 @@
         <v>2</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F22" s="23">
         <v>768</v>
@@ -2308,7 +2311,7 @@
         <v>2</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F23" s="23">
         <v>768</v>
@@ -2362,7 +2365,7 @@
         <v>2</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F24" s="23">
         <v>768</v>
@@ -2416,7 +2419,7 @@
         <v>2</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F25" s="23">
         <v>768</v>
@@ -2470,7 +2473,7 @@
         <v>2</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F26" s="23">
         <v>768</v>
@@ -2524,7 +2527,7 @@
         <v>2</v>
       </c>
       <c r="E27" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F27" s="23">
         <v>768</v>
@@ -2578,7 +2581,7 @@
         <v>2</v>
       </c>
       <c r="E28" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F28" s="23">
         <v>768</v>
@@ -2633,7 +2636,7 @@
         <v>2</v>
       </c>
       <c r="E29" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F29" s="23">
         <v>768</v>
@@ -2688,7 +2691,7 @@
         <v>2</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F30" s="23">
         <v>768</v>
@@ -2742,7 +2745,7 @@
         <v>2</v>
       </c>
       <c r="E31" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F31" s="23">
         <v>768</v>
@@ -2796,7 +2799,7 @@
         <v>2</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F32" s="23">
         <v>768</v>
@@ -2850,7 +2853,7 @@
         <v>2</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F33" s="23">
         <v>768</v>
@@ -2904,7 +2907,7 @@
         <v>2</v>
       </c>
       <c r="E34" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F34" s="23">
         <v>768</v>
@@ -2958,7 +2961,7 @@
         <v>2</v>
       </c>
       <c r="E35" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F35" s="23">
         <v>768</v>
@@ -3012,7 +3015,7 @@
         <v>2</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F36" s="23">
         <v>768</v>
@@ -3067,7 +3070,7 @@
         <v>2</v>
       </c>
       <c r="E37" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F37" s="23">
         <v>768</v>
@@ -3121,7 +3124,7 @@
         <v>2</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F38" s="23">
         <v>768</v>
@@ -3175,7 +3178,7 @@
         <v>2</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F39" s="23">
         <v>768</v>
@@ -3229,7 +3232,7 @@
         <v>2</v>
       </c>
       <c r="E40" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F40" s="23">
         <v>768</v>
@@ -3284,7 +3287,7 @@
         <v>2</v>
       </c>
       <c r="E41" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F41" s="23">
         <v>512</v>
@@ -3339,7 +3342,7 @@
         <v>2</v>
       </c>
       <c r="E42" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F42" s="23">
         <v>768</v>
@@ -3393,7 +3396,7 @@
         <v>2</v>
       </c>
       <c r="E43" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F43" s="23">
         <v>768</v>
@@ -3447,7 +3450,7 @@
         <v>2</v>
       </c>
       <c r="E44" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F44" s="23">
         <v>512</v>
@@ -3501,7 +3504,7 @@
         <v>2</v>
       </c>
       <c r="E45" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F45" s="23">
         <v>512</v>
@@ -3555,7 +3558,7 @@
         <v>2</v>
       </c>
       <c r="E46" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F46" s="23">
         <v>512</v>
@@ -3609,7 +3612,7 @@
         <v>2</v>
       </c>
       <c r="E47" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F47" s="23">
         <v>512</v>
@@ -3664,7 +3667,7 @@
         <v>2</v>
       </c>
       <c r="E48" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F48" s="23">
         <v>512</v>
@@ -3709,7 +3712,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="49" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B49" s="20" t="s">
         <v>4</v>
       </c>
@@ -3720,7 +3723,7 @@
         <v>2</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F49" s="23">
         <v>512</v>
@@ -3747,10 +3750,10 @@
       <c r="Q49" s="30"/>
       <c r="R49" s="30"/>
       <c r="T49" s="56" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="50" spans="1:21" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="50" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
         <v>4</v>
       </c>
@@ -3761,7 +3764,7 @@
         <v>2</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F50" s="23">
         <v>512</v>
@@ -3800,7 +3803,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="51" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
         <v>4</v>
       </c>
@@ -3811,7 +3814,7 @@
         <v>2</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F51" s="23">
         <v>512</v>
@@ -3850,7 +3853,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="52" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
         <v>4</v>
       </c>
@@ -3861,7 +3864,7 @@
         <v>2</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F52" s="23">
         <v>512</v>
@@ -3900,7 +3903,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="53" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
         <v>4</v>
       </c>
@@ -3911,7 +3914,7 @@
         <v>2</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F53" s="23">
         <v>512</v>
@@ -3950,7 +3953,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="54" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
         <v>4</v>
       </c>
@@ -3961,7 +3964,7 @@
         <v>2</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F54" s="23">
         <v>512</v>
@@ -4000,7 +4003,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="55" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
         <v>4</v>
       </c>
@@ -4011,7 +4014,7 @@
         <v>2</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F55" s="23">
         <v>512</v>
@@ -4050,7 +4053,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="56" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
         <v>4</v>
       </c>
@@ -4061,7 +4064,7 @@
         <v>2</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F56" s="23">
         <v>512</v>
@@ -4100,7 +4103,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="57" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:22" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="1"/>
       <c r="B57" s="40" t="s">
         <v>4</v>
@@ -4112,7 +4115,7 @@
         <v>2</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F57" s="23">
         <v>512</v>
@@ -4154,7 +4157,7 @@
       <c r="S57" s="49"/>
       <c r="U57" s="19"/>
     </row>
-    <row r="58" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
         <v>4</v>
       </c>
@@ -4165,7 +4168,7 @@
         <v>2</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F58" s="23">
         <v>512</v>
@@ -4204,7 +4207,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="59" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B59" s="40" t="s">
         <v>4</v>
       </c>
@@ -4215,7 +4218,7 @@
         <v>2</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F59" s="23">
         <v>512</v>
@@ -4254,7 +4257,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="60" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B60" s="40" t="s">
         <v>4</v>
       </c>
@@ -4265,7 +4268,7 @@
         <v>2</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F60" s="23">
         <v>512</v>
@@ -4304,7 +4307,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="61" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B61" s="40" t="s">
         <v>4</v>
       </c>
@@ -4315,7 +4318,7 @@
         <v>2</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F61" s="23">
         <v>512</v>
@@ -4354,7 +4357,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="62" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B62" s="40" t="s">
         <v>4</v>
       </c>
@@ -4365,7 +4368,7 @@
         <v>2</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F62" s="23">
         <v>512</v>
@@ -4404,7 +4407,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="63" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:22" x14ac:dyDescent="0.25">
       <c r="B63" s="40" t="s">
         <v>4</v>
       </c>
@@ -4415,7 +4418,7 @@
         <v>2</v>
       </c>
       <c r="E63" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F63" s="23">
         <v>512</v>
@@ -4454,7 +4457,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="64" spans="1:21" s="18" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:22" s="18" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="1"/>
       <c r="B64" s="40" t="s">
         <v>4</v>
@@ -4466,7 +4469,7 @@
         <v>2</v>
       </c>
       <c r="E64" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F64" s="23">
         <v>512</v>
@@ -4488,25 +4491,37 @@
       </c>
       <c r="L64" s="19"/>
       <c r="M64" s="36">
+        <f>160*$V64</f>
         <v>160</v>
       </c>
-      <c r="N64" s="32">
+      <c r="N64" s="19">
+        <f>165*$V64</f>
         <v>165</v>
       </c>
-      <c r="O64" s="32">
+      <c r="O64" s="19">
+        <f>252*$V64</f>
         <v>252</v>
       </c>
       <c r="P64" s="36">
+        <f>570*$V64</f>
         <v>570</v>
       </c>
-      <c r="Q64" s="44">
+      <c r="Q64" s="19">
+        <f>181*$V64</f>
         <v>181</v>
       </c>
-      <c r="R64" s="44">
+      <c r="R64" s="19">
+        <f>252*$V64</f>
         <v>252</v>
       </c>
       <c r="S64" s="49"/>
+      <c r="T64" s="18" t="s">
+        <v>119</v>
+      </c>
       <c r="U64" s="19"/>
+      <c r="V64" s="18">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="2:18" x14ac:dyDescent="0.25">
       <c r="B65" s="40" t="s">
@@ -4519,7 +4534,7 @@
         <v>2</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F65" s="23">
         <v>512</v>
@@ -4569,7 +4584,7 @@
         <v>2</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F66" s="23">
         <v>512</v>
@@ -4619,7 +4634,7 @@
         <v>2</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F67" s="23">
         <v>512</v>
@@ -4669,7 +4684,7 @@
         <v>2</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F68" s="23">
         <v>512</v>
@@ -4719,7 +4734,7 @@
         <v>2</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F69" s="23">
         <v>512</v>
@@ -4769,7 +4784,7 @@
         <v>2</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F70" s="23">
         <v>512</v>
@@ -4819,7 +4834,7 @@
         <v>2</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F71" s="23">
         <v>512</v>
@@ -4869,7 +4884,7 @@
         <v>2</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F72" s="23">
         <v>512</v>
@@ -4919,7 +4934,7 @@
         <v>2</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F73" s="23">
         <v>512</v>
@@ -4969,7 +4984,7 @@
         <v>2</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F74" s="23">
         <v>512</v>
@@ -5019,7 +5034,7 @@
         <v>2</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F75" s="23">
         <v>512</v>
@@ -5069,7 +5084,7 @@
         <v>2</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F76" s="23">
         <v>512</v>
@@ -5119,7 +5134,7 @@
         <v>2</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F77" s="23">
         <v>512</v>
@@ -5169,7 +5184,7 @@
         <v>2</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F78" s="23">
         <v>512</v>
@@ -5219,7 +5234,7 @@
         <v>2</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F79" s="23">
         <v>512</v>
@@ -5269,7 +5284,7 @@
         <v>2</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F80" s="23">
         <v>512</v>
@@ -5319,7 +5334,7 @@
         <v>2</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F81" s="23">
         <v>512</v>
@@ -5340,19 +5355,19 @@
         <v>0.5</v>
       </c>
       <c r="M81" s="34">
-        <v>158</v>
+        <v>91</v>
       </c>
       <c r="N81" s="30">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="O81" s="30">
         <v>262</v>
       </c>
       <c r="P81" s="34">
-        <v>680</v>
+        <v>632</v>
       </c>
       <c r="Q81" s="30">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="R81" s="30">
         <v>262</v>
@@ -5370,7 +5385,7 @@
         <v>2</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F82" s="23">
         <v>512</v>
@@ -5421,7 +5436,7 @@
         <v>2</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F83" s="23">
         <v>512</v>
@@ -5472,10 +5487,10 @@
         <v>90</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>92</v>
+        <v>2</v>
       </c>
       <c r="E84" s="17" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F84" s="25">
         <v>512</v>
@@ -5525,10 +5540,10 @@
         <v>6</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E85" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F85" s="23">
         <v>768</v>
@@ -5581,10 +5596,10 @@
         <v>7</v>
       </c>
       <c r="D86" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E86" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F86" s="23">
         <v>768</v>
@@ -5637,10 +5652,10 @@
         <v>8</v>
       </c>
       <c r="D87" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E87" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F87" s="23">
         <v>768</v>
@@ -5693,10 +5708,10 @@
         <v>84</v>
       </c>
       <c r="D88" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E88" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F88" s="23">
         <v>768</v>
@@ -5749,10 +5764,10 @@
         <v>9</v>
       </c>
       <c r="D89" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E89" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F89" s="23">
         <v>768</v>
@@ -5805,10 +5820,10 @@
         <v>10</v>
       </c>
       <c r="D90" s="67" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="E90" s="68" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I90" s="24"/>
       <c r="J90" s="24"/>
@@ -5820,7 +5835,7 @@
       <c r="Q90" s="30"/>
       <c r="R90" s="30"/>
       <c r="T90" s="69" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="U90" s="70">
         <v>205.5</v>
@@ -5834,10 +5849,10 @@
         <v>85</v>
       </c>
       <c r="D91" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E91" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F91" s="23">
         <v>768</v>
@@ -5890,10 +5905,10 @@
         <v>11</v>
       </c>
       <c r="D92" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E92" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F92" s="23">
         <v>768</v>
@@ -5946,10 +5961,10 @@
         <v>12</v>
       </c>
       <c r="D93" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E93" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F93" s="23">
         <v>768</v>
@@ -6002,10 +6017,10 @@
         <v>13</v>
       </c>
       <c r="D94" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E94" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F94" s="23">
         <v>768</v>
@@ -6058,10 +6073,10 @@
         <v>14</v>
       </c>
       <c r="D95" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E95" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F95" s="23">
         <v>768</v>
@@ -6114,10 +6129,10 @@
         <v>15</v>
       </c>
       <c r="D96" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E96" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F96" s="23">
         <v>768</v>
@@ -6170,10 +6185,10 @@
         <v>16</v>
       </c>
       <c r="D97" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E97" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F97" s="23">
         <v>768</v>
@@ -6226,10 +6241,10 @@
         <v>17</v>
       </c>
       <c r="D98" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E98" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F98" s="23">
         <v>768</v>
@@ -6282,10 +6297,10 @@
         <v>18</v>
       </c>
       <c r="D99" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E99" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F99" s="23">
         <v>768</v>
@@ -6338,10 +6353,10 @@
         <v>19</v>
       </c>
       <c r="D100" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E100" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F100" s="23">
         <v>768</v>
@@ -6394,10 +6409,10 @@
         <v>20</v>
       </c>
       <c r="D101" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E101" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F101" s="23">
         <v>768</v>
@@ -6450,10 +6465,10 @@
         <v>21</v>
       </c>
       <c r="D102" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E102" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F102" s="23">
         <v>768</v>
@@ -6506,10 +6521,10 @@
         <v>22</v>
       </c>
       <c r="D103" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E103" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F103" s="23">
         <v>768</v>
@@ -6562,10 +6577,10 @@
         <v>23</v>
       </c>
       <c r="D104" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E104" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F104" s="23">
         <v>768</v>
@@ -6618,10 +6633,10 @@
         <v>24</v>
       </c>
       <c r="D105" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E105" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F105" s="23">
         <v>768</v>
@@ -6674,10 +6689,10 @@
         <v>25</v>
       </c>
       <c r="D106" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E106" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F106" s="23">
         <v>768</v>
@@ -6730,10 +6745,10 @@
         <v>26</v>
       </c>
       <c r="D107" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E107" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F107" s="23">
         <v>768</v>
@@ -6786,10 +6801,10 @@
         <v>27</v>
       </c>
       <c r="D108" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E108" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F108" s="23">
         <v>768</v>
@@ -6842,10 +6857,10 @@
         <v>28</v>
       </c>
       <c r="D109" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E109" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F109" s="23">
         <v>768</v>
@@ -6898,10 +6913,10 @@
         <v>29</v>
       </c>
       <c r="D110" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E110" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F110" s="23">
         <v>768</v>
@@ -6954,10 +6969,10 @@
         <v>30</v>
       </c>
       <c r="D111" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E111" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F111" s="23">
         <v>768</v>
@@ -7010,10 +7025,10 @@
         <v>31</v>
       </c>
       <c r="D112" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E112" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F112" s="23">
         <v>768</v>
@@ -7058,7 +7073,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="113" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B113" t="s">
         <v>3</v>
       </c>
@@ -7066,10 +7081,10 @@
         <v>86</v>
       </c>
       <c r="D113" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E113" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F113" s="23">
         <v>768</v>
@@ -7114,7 +7129,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="114" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B114" t="s">
         <v>3</v>
       </c>
@@ -7122,10 +7137,10 @@
         <v>32</v>
       </c>
       <c r="D114" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E114" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F114" s="23">
         <v>768</v>
@@ -7170,7 +7185,7 @@
         <v>185.5</v>
       </c>
     </row>
-    <row r="115" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B115" t="s">
         <v>3</v>
       </c>
@@ -7178,10 +7193,10 @@
         <v>33</v>
       </c>
       <c r="D115" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E115" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F115" s="23">
         <v>768</v>
@@ -7226,7 +7241,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="116" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B116" t="s">
         <v>3</v>
       </c>
@@ -7234,10 +7249,10 @@
         <v>34</v>
       </c>
       <c r="D116" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E116" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F116" s="23">
         <v>768</v>
@@ -7282,7 +7297,7 @@
         <v>245</v>
       </c>
     </row>
-    <row r="117" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B117" t="s">
         <v>3</v>
       </c>
@@ -7290,10 +7305,10 @@
         <v>35</v>
       </c>
       <c r="D117" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E117" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F117" s="23">
         <v>768</v>
@@ -7338,7 +7353,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="118" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B118" t="s">
         <v>3</v>
       </c>
@@ -7346,10 +7361,10 @@
         <v>36</v>
       </c>
       <c r="D118" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E118" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F118" s="23">
         <v>768</v>
@@ -7394,7 +7409,7 @@
         <v>224.5</v>
       </c>
     </row>
-    <row r="119" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B119" t="s">
         <v>3</v>
       </c>
@@ -7402,10 +7417,10 @@
         <v>41</v>
       </c>
       <c r="D119" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E119" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F119" s="23">
         <v>768</v>
@@ -7450,7 +7465,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="120" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B120" t="s">
         <v>3</v>
       </c>
@@ -7458,10 +7473,10 @@
         <v>37</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E120" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F120" s="23">
         <v>768</v>
@@ -7506,7 +7521,7 @@
         <v>218.5</v>
       </c>
     </row>
-    <row r="121" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B121" t="s">
         <v>3</v>
       </c>
@@ -7514,10 +7529,10 @@
         <v>42</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E121" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F121" s="23">
         <v>768</v>
@@ -7562,7 +7577,7 @@
         <v>247</v>
       </c>
     </row>
-    <row r="122" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
         <v>3</v>
       </c>
@@ -7570,10 +7585,10 @@
         <v>43</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E122" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F122" s="23">
         <v>768</v>
@@ -7618,10 +7633,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="123" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A123" s="1">
-        <v>1</v>
-      </c>
+    <row r="123" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
         <v>3</v>
       </c>
@@ -7629,10 +7641,10 @@
         <v>87</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E123" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F123" s="23">
         <v>768</v>
@@ -7677,7 +7689,7 @@
         <v>208.5</v>
       </c>
     </row>
-    <row r="124" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
         <v>3</v>
       </c>
@@ -7685,10 +7697,10 @@
         <v>88</v>
       </c>
       <c r="D124" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E124" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F124" s="23">
         <v>768</v>
@@ -7733,7 +7745,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="125" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
         <v>3</v>
       </c>
@@ -7741,10 +7753,10 @@
         <v>44</v>
       </c>
       <c r="D125" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E125" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F125" s="23">
         <v>768</v>
@@ -7789,7 +7801,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="126" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
         <v>3</v>
       </c>
@@ -7797,10 +7809,10 @@
         <v>45</v>
       </c>
       <c r="D126" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E126" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F126" s="23">
         <v>768</v>
@@ -7845,7 +7857,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="127" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
         <v>3</v>
       </c>
@@ -7853,10 +7865,10 @@
         <v>89</v>
       </c>
       <c r="D127" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E127" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F127" s="23">
         <v>512</v>
@@ -7901,7 +7913,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="128" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
         <v>3</v>
       </c>
@@ -7909,10 +7921,10 @@
         <v>38</v>
       </c>
       <c r="D128" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E128" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F128" s="23">
         <v>512</v>
@@ -7965,10 +7977,10 @@
         <v>39</v>
       </c>
       <c r="D129" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E129" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F129" s="23">
         <v>512</v>
@@ -8021,10 +8033,10 @@
         <v>46</v>
       </c>
       <c r="D130" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E130" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F130" s="23">
         <v>512</v>
@@ -8078,10 +8090,10 @@
         <v>40</v>
       </c>
       <c r="D131" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E131" s="13" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F131" s="23">
         <v>512</v>
@@ -8139,7 +8151,7 @@
         <v>83</v>
       </c>
       <c r="E132" s="65" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="I132" s="24"/>
       <c r="J132" s="24"/>
@@ -8151,7 +8163,7 @@
       <c r="Q132" s="30"/>
       <c r="R132" s="30"/>
       <c r="T132" s="58" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="133" spans="1:21" x14ac:dyDescent="0.25">
@@ -8162,10 +8174,10 @@
         <v>48</v>
       </c>
       <c r="D133" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E133" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F133" s="23">
         <v>512</v>
@@ -8212,10 +8224,10 @@
         <v>49</v>
       </c>
       <c r="D134" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E134" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F134" s="23">
         <v>512</v>
@@ -8262,10 +8274,10 @@
         <v>50</v>
       </c>
       <c r="D135" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E135" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F135" s="23">
         <v>512</v>
@@ -8312,10 +8324,10 @@
         <v>51</v>
       </c>
       <c r="D136" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E136" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F136" s="23">
         <v>512</v>
@@ -8362,10 +8374,10 @@
         <v>52</v>
       </c>
       <c r="D137" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E137" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F137" s="23">
         <v>512</v>
@@ -8412,10 +8424,10 @@
         <v>53</v>
       </c>
       <c r="D138" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E138" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F138" s="23">
         <v>512</v>
@@ -8462,10 +8474,10 @@
         <v>54</v>
       </c>
       <c r="D139" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E139" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F139" s="23">
         <v>512</v>
@@ -8512,10 +8524,10 @@
         <v>55</v>
       </c>
       <c r="D140" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E140" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F140" s="23">
         <v>512</v>
@@ -8562,10 +8574,10 @@
         <v>56</v>
       </c>
       <c r="D141" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E141" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F141" s="23">
         <v>512</v>
@@ -8612,10 +8624,10 @@
         <v>57</v>
       </c>
       <c r="D142" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E142" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F142" s="23">
         <v>512</v>
@@ -8662,10 +8674,10 @@
         <v>58</v>
       </c>
       <c r="D143" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E143" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F143" s="23">
         <v>512</v>
@@ -8691,7 +8703,7 @@
       <c r="Q143" s="30"/>
       <c r="R143" s="30"/>
       <c r="T143" s="59" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="144" spans="1:21" x14ac:dyDescent="0.25">
@@ -8702,10 +8714,10 @@
         <v>59</v>
       </c>
       <c r="D144" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E144" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F144" s="23">
         <v>512</v>
@@ -8752,10 +8764,10 @@
         <v>60</v>
       </c>
       <c r="D145" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E145" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F145" s="23">
         <v>512</v>
@@ -8802,10 +8814,10 @@
         <v>61</v>
       </c>
       <c r="D146" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E146" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F146" s="23">
         <v>512</v>
@@ -8852,10 +8864,10 @@
         <v>62</v>
       </c>
       <c r="D147" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E147" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F147" s="23">
         <v>512</v>
@@ -8903,10 +8915,10 @@
         <v>63</v>
       </c>
       <c r="D148" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E148" s="42" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F148" s="23">
         <v>512</v>
@@ -8953,10 +8965,10 @@
         <v>64</v>
       </c>
       <c r="D149" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E149" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F149" s="23">
         <v>512</v>
@@ -9003,10 +9015,10 @@
         <v>65</v>
       </c>
       <c r="D150" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E150" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F150" s="23">
         <v>512</v>
@@ -9053,7 +9065,7 @@
         <v>66</v>
       </c>
       <c r="D151" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E151" s="42"/>
       <c r="I151" s="24"/>
@@ -9066,7 +9078,7 @@
       <c r="Q151" s="30"/>
       <c r="R151" s="30"/>
       <c r="T151" s="60" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="152" spans="2:20" x14ac:dyDescent="0.25">
@@ -9077,10 +9089,10 @@
         <v>67</v>
       </c>
       <c r="D152" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E152" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F152" s="23">
         <v>512</v>
@@ -9127,10 +9139,10 @@
         <v>68</v>
       </c>
       <c r="D153" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E153" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F153" s="23">
         <v>512</v>
@@ -9177,10 +9189,10 @@
         <v>69</v>
       </c>
       <c r="D154" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E154" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F154" s="23">
         <v>512</v>
@@ -9227,10 +9239,10 @@
         <v>70</v>
       </c>
       <c r="D155" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E155" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F155" s="23">
         <v>512</v>
@@ -9277,10 +9289,10 @@
         <v>71</v>
       </c>
       <c r="D156" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E156" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F156" s="23">
         <v>512</v>
@@ -9327,10 +9339,10 @@
         <v>72</v>
       </c>
       <c r="D157" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E157" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F157" s="23">
         <v>512</v>
@@ -9377,10 +9389,10 @@
         <v>73</v>
       </c>
       <c r="D158" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E158" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F158" s="23">
         <v>512</v>
@@ -9427,10 +9439,10 @@
         <v>74</v>
       </c>
       <c r="D159" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E159" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F159" s="23">
         <v>512</v>
@@ -9477,10 +9489,10 @@
         <v>75</v>
       </c>
       <c r="D160" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E160" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F160" s="23">
         <v>512</v>
@@ -9527,10 +9539,10 @@
         <v>76</v>
       </c>
       <c r="D161" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E161" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F161" s="23">
         <v>512</v>
@@ -9577,10 +9589,10 @@
         <v>77</v>
       </c>
       <c r="D162" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E162" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F162" s="23">
         <v>512</v>
@@ -9627,10 +9639,10 @@
         <v>78</v>
       </c>
       <c r="D163" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E163" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F163" s="23">
         <v>512</v>
@@ -9677,10 +9689,10 @@
         <v>79</v>
       </c>
       <c r="D164" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E164" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F164" s="23">
         <v>512</v>
@@ -9719,7 +9731,7 @@
         <v>260</v>
       </c>
       <c r="T164" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="165" spans="2:20" x14ac:dyDescent="0.25">
@@ -9730,10 +9742,10 @@
         <v>80</v>
       </c>
       <c r="D165" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E165" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F165" s="23">
         <v>512</v>
@@ -9780,10 +9792,10 @@
         <v>81</v>
       </c>
       <c r="D166" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E166" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F166" s="23">
         <v>512</v>
@@ -9830,10 +9842,10 @@
         <v>90</v>
       </c>
       <c r="D167" s="54" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E167" s="42" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="F167" s="23">
         <v>512</v>

</xml_diff>